<commit_message>
Updated DarkATP solution recipe
Added in Purity percentages for current chemical stock
</commit_message>
<xml_diff>
--- a/Solution_recipes/Pulse_Chase_solutions/DarkATP_template.xlsx
+++ b/Solution_recipes/Pulse_Chase_solutions/DarkATP_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg Milburn\Documents\solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Solution_recipes\Pulse_Chase_solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CD835A9-4DE7-484D-B144-45588AAD898F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC3629B-EAE4-4D27-ADC3-C639DD27328A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,22 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$17</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -96,9 +83,6 @@
   </si>
   <si>
     <t>Target pH = 6.80</t>
-  </si>
-  <si>
-    <t>Catelog</t>
   </si>
   <si>
     <t>MgCl2 Stock Solution</t>
@@ -202,6 +186,9 @@
       <t xml:space="preserve"> unless explicitly stated </t>
     </r>
   </si>
+  <si>
+    <t>Catalog</t>
+  </si>
 </sst>
 </file>
 
@@ -209,8 +196,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -573,24 +560,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,16 +587,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -639,13 +614,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -654,10 +629,7 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -667,17 +639,32 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,7 +987,7 @@
   <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1020,113 +1007,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="A1" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
     </row>
     <row r="5" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="C5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="28" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1137,32 +1124,34 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="33">
+      <c r="E6" s="29">
         <v>209.26329999999999</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="33" t="e">
-        <f t="shared" ref="G6:G7" si="0">E6/F6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" s="12">
+      <c r="F6" s="22">
+        <v>0.995</v>
+      </c>
+      <c r="G6" s="29">
+        <f>E6/F6</f>
+        <v>210.31487437185928</v>
+      </c>
+      <c r="H6" s="45">
         <v>0.05</v>
       </c>
-      <c r="I6" s="34" t="e">
+      <c r="I6" s="30">
         <f>G6*H6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J6" s="34" t="e">
-        <f t="shared" ref="J6:J12" si="1">I6/2</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K6" s="34" t="e">
+        <v>10.515743718592965</v>
+      </c>
+      <c r="J6" s="30">
+        <f t="shared" ref="J6:J12" si="0">I6/2</f>
+        <v>5.2578718592964826</v>
+      </c>
+      <c r="K6" s="30">
         <f>I6*0.25</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L6" s="34" t="e">
+        <v>2.6289359296482413</v>
+      </c>
+      <c r="L6" s="30">
         <f>I6*0.1</f>
-        <v>#DIV/0!</v>
+        <v>1.0515743718592965</v>
       </c>
       <c r="M6" s="8"/>
     </row>
@@ -1173,32 +1162,34 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="33">
+      <c r="E7" s="29">
         <v>98.15</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="33" t="e">
+      <c r="F7" s="22">
+        <v>0.99</v>
+      </c>
+      <c r="G7" s="29">
+        <f t="shared" ref="G6:G7" si="1">E7/F7</f>
+        <v>99.141414141414145</v>
+      </c>
+      <c r="H7" s="45">
+        <v>0.12</v>
+      </c>
+      <c r="I7" s="30">
+        <f>G7*H7</f>
+        <v>11.896969696969697</v>
+      </c>
+      <c r="J7" s="30">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="I7" s="34" t="e">
-        <f>G7*H7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J7" s="34" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K7" s="34" t="e">
+        <v>5.9484848484848483</v>
+      </c>
+      <c r="K7" s="30">
         <f t="shared" ref="K7:K12" si="2">I7*0.25</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L7" s="34" t="e">
+        <v>2.9742424242424241</v>
+      </c>
+      <c r="L7" s="30">
         <f t="shared" ref="L7:L12" si="3">I7*0.1</f>
-        <v>#DIV/0!</v>
+        <v>1.1896969696969697</v>
       </c>
       <c r="M7" s="8"/>
     </row>
@@ -1212,238 +1203,244 @@
       <c r="E8" s="2">
         <v>380.35</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="33" t="e">
+      <c r="F8" s="22">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="G8" s="29">
         <f>E8/F8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="12">
+        <v>388.50868232890707</v>
+      </c>
+      <c r="H8" s="45">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I8" s="34" t="e">
+      <c r="I8" s="30">
         <f>G8*H8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J8" s="34" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" s="34" t="e">
+        <v>1.9425434116445355</v>
+      </c>
+      <c r="J8" s="30">
+        <f t="shared" si="0"/>
+        <v>0.97127170582226774</v>
+      </c>
+      <c r="K8" s="30">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L8" s="34" t="e">
+        <v>0.48563585291113387</v>
+      </c>
+      <c r="L8" s="30">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.19425434116445356</v>
       </c>
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14">
+      <c r="B9" s="13"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13">
         <v>154.25299999999999</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="33" t="e">
+      <c r="F9" s="22">
+        <v>0.99</v>
+      </c>
+      <c r="G9" s="29">
         <f>E9/F9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="15">
+        <v>155.8111111111111</v>
+      </c>
+      <c r="H9" s="46">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I9" s="34" t="e">
+      <c r="I9" s="30">
         <f>G9*H9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" s="34" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="34" t="e">
+        <v>0.62324444444444438</v>
+      </c>
+      <c r="J9" s="30">
+        <f t="shared" si="0"/>
+        <v>0.31162222222222219</v>
+      </c>
+      <c r="K9" s="30">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L9" s="34" t="e">
+        <v>0.15581111111111109</v>
+      </c>
+      <c r="L9" s="30">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M9" s="16"/>
+        <v>6.2324444444444439E-2</v>
+      </c>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14">
+      <c r="A10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13">
         <v>136.08600000000001</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="33" t="e">
+      <c r="F10" s="23">
+        <v>0.99</v>
+      </c>
+      <c r="G10" s="29">
         <f>E10/F10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" s="15">
+        <v>137.46060606060607</v>
+      </c>
+      <c r="H10" s="46">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I10" s="34" t="e">
+      <c r="I10" s="30">
         <f>G10*H10</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" s="34" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="34" t="e">
+        <v>0.6873030303030303</v>
+      </c>
+      <c r="J10" s="30">
+        <f t="shared" si="0"/>
+        <v>0.34365151515151515</v>
+      </c>
+      <c r="K10" s="30">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="34" t="e">
+        <v>0.17182575757575758</v>
+      </c>
+      <c r="L10" s="30">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>6.873030303030303E-2</v>
       </c>
       <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="15">
+      <c r="A11" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="46">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="16"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="38">
+      <c r="A12" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="34">
         <v>0.5</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="47">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="35">
         <f>((H12*1)/G12)*1000</f>
         <v>10</v>
       </c>
-      <c r="J12" s="39">
-        <f t="shared" si="1"/>
+      <c r="J12" s="35">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="K12" s="39">
+      <c r="K12" s="35">
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="L12" s="39">
+      <c r="L12" s="35">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M12" s="25"/>
+      <c r="M12" s="21"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:13" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
     </row>
     <row r="17" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
     </row>
     <row r="40" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="45" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1476,11 +1473,20 @@
     <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="74" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<LabArchives xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema">
+  <BaseUri>https://mynotebook.labarchives.com</BaseUri>
+  <eid>MTQ1OC42MDAwMDAwMDAwMDAxfDY3MzMyMS8xMTIyL0VudHJ5UGFydC8xNDk3MTQxNTg1fDM3MDIuNg==</eid>
+  <version>1</version>
+  <updated-at>2023-02-07T15:12:20Z</updated-at>
+</LabArchives>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abfa450e2c882fa05ec7f6a4b4016779">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53678093842f3275b6926b32e7a9c141" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -1703,22 +1709,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LabArchives xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema">
-  <BaseUri>https://mynotebook.labarchives.com</BaseUri>
-  <eid>MTQ1OC42MDAwMDAwMDAwMDAxfDY3MzMyMS8xMTIyL0VudHJ5UGFydC8xNDk3MTQxNTg1fDM3MDIuNg==</eid>
-  <version>1</version>
-  <updated-at>2023-02-07T15:12:20Z</updated-at>
-</LabArchives>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1727,7 +1718,21 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF7C2CCE-8D20-4A3D-AD69-72DDEBC247C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A5D5A9-477B-4B97-9F9B-D797D2834A6C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1746,15 +1751,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF7C2CCE-8D20-4A3D-AD69-72DDEBC247C7}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576E4525-D34E-471F-91EB-AF7A16356FDF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3012E31E-5C99-4C5B-9323-B5D42B3C4F74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1769,12 +1774,4 @@
     <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576E4525-D34E-471F-91EB-AF7A16356FDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>